<commit_message>
%ise au point du transcodage WWO vers Weather.com
git-svn-id: svn://zone.spip.org/spip-zone/_plugins_@122898 ac52e18a-acf5-0310-9fe8-c4428f23b10a
</commit_message>
<xml_diff>
--- a/rainette/trunk/themes/codes.xlsx
+++ b/rainette/trunk/themes/codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/Sites/SPIP/plugins/rainette/themes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DC7CAB-ADED-404F-B684-B9861BBFFF51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7AD336-C953-7C41-A4E0-8C24BE802A13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37820" yWindow="460" windowWidth="32300" windowHeight="22280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1547,30 +1547,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH967"/>
+  <dimension ref="A1:AB967"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="5.6640625" style="3" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="24.6640625" style="3" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="30.83203125" style="3" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="4.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="31.83203125" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="10.83203125" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="4.83203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="6" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="32.5" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="5.83203125" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="7.5" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="5.1640625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22" style="3" customWidth="1"/>
-    <col min="16" max="16" width="5.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="31.83203125" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="10.83203125" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="4.83203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="6" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="32.5" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="5.83203125" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="7.5" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="5.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="22" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="5.1640625" style="3" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="6" style="3" customWidth="1" outlineLevel="1"/>
     <col min="18" max="18" width="44.83203125" style="3" customWidth="1" outlineLevel="1"/>
     <col min="19" max="19" width="41.1640625" style="3" customWidth="1" outlineLevel="1"/>

</xml_diff>